<commit_message>
Added figures and jupyter notebook plots of bar chart for the ablation study
</commit_message>
<xml_diff>
--- a/reports/Excels/3_Ablation_study_drop_one.xlsx
+++ b/reports/Excels/3_Ablation_study_drop_one.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orelt\projects\Sleep-Stage-Prediction-Classification-Using-Neural-ODE\reports\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9CBDAB-A348-4A4C-8427-927C2EFAE3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594E5EEA-22C7-4370-B673-B2A3B9BC57EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31188" yWindow="468" windowWidth="21612" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31656" yWindow="936" windowWidth="21612" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
     <sheet name="summary" sheetId="2" r:id="rId2"/>
+    <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>SC4001E0</t>
   </si>
@@ -154,7 +155,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +196,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,8 +249,18 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -320,6 +356,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -332,14 +383,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -349,19 +403,25 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="6" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="7" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="הערה" xfId="4" builtinId="10"/>
     <cellStyle name="חישוב" xfId="2" builtinId="22"/>
     <cellStyle name="טוב" xfId="1" builtinId="26"/>
+    <cellStyle name="ניטראלי" xfId="6" builtinId="28"/>
+    <cellStyle name="פלט" xfId="7" builtinId="21"/>
+    <cellStyle name="רע" xfId="5" builtinId="27"/>
     <cellStyle name="תא מסומן" xfId="3" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,26 +721,26 @@
   <sheetData>
     <row r="1" spans="2:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="10"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="2:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
@@ -1394,7 +1454,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1413,34 +1473,34 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1553,4 +1613,179 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD45B32-C267-4549-919C-7CB05DDBF42E}">
+  <dimension ref="F3:I13"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="11">
+        <v>3.2624606364301686E-2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.98756497290609102</v>
+      </c>
+    </row>
+    <row r="5" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="11">
+        <v>5.0047107008590629E-2</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.78181400141743884</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.78981847902535485</v>
+      </c>
+    </row>
+    <row r="6" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.26217077641475905</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.53666375411268397</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.63922080510769241</v>
+      </c>
+    </row>
+    <row r="7" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0.16240387885763227</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.53497615262321108</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.55390715161951065</v>
+      </c>
+    </row>
+    <row r="8" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="11">
+        <v>3.1412526615428302E-2</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.98410487348820752</v>
+      </c>
+    </row>
+    <row r="9" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="11">
+        <v>5.1471660157878865E-2</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.80736725663716802</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.79272985558212639</v>
+      </c>
+    </row>
+    <row r="10" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.1052961570440222</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.97056113686150713</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="11">
+        <v>9.6232077787066148E-2</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0.77628529287821246</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.76081292832026759</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="11">
+        <v>2.441409349934474E-2</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.99182843856530156</v>
+      </c>
+    </row>
+    <row r="13" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="11">
+        <v>4.4574302551752196E-2</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.78153739371854902</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.77497170739837218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>